<commit_message>
Update daily driver report to include more employee information
Updates daily report JSON, XLSX, and PDF files, and adds a trend report JSON file.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: b83b866c-5b8f-4d82-9fde-612e7a355315
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/f2699832-8135-4557-9ec0-8d4d723b9ba2/b41737f0-74b2-42b4-a76f-b628ea244f23.jpg
</commit_message>
<xml_diff>
--- a/exports/daily_reports/2025-05-20_DailyDriverReport.xlsx
+++ b/exports/daily_reports/2025-05-20_DailyDriverReport.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,20 +441,45 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>employee_id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>phone</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>division</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>job_title</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>asset</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>arrival</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>departure</t>
         </is>
@@ -463,305 +488,1522 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>John Smith</t>
+          <t>Humberto Esparza-Camos</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>RAM-2500</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>On Time</t>
-        </is>
-      </c>
+          <t>240276</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>07:00 AM</t>
+          <t>(817) 769-0088</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>F-35</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>06:49 AM</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Mary Johnson</t>
+          <t>Kevin Martinez</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>F-150</t>
+          <t>240732</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>On Time</t>
+          <t>kevinm469@icloud.com</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>07:15 AM</t>
+          <t>(817) 730-1024</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>ET-95</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>07:11 AM</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Robert Williams</t>
+          <t>Otoniel Onofre-Alas</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ET-05</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
+          <t>240281</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>(817) 812-8023</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>RAM-62</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
         <is>
           <t>Late</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>08:30 AM</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>07:45 AM</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Patricia Brown</t>
+          <t>Edgar Cabrera-Moreno</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>RAM-3500</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>On Time</t>
-        </is>
-      </c>
+          <t>440127</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>07:10 AM</t>
+          <t>(409) 229-6071</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>HD-78</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>07:24 AM</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Michael Davis</t>
+          <t>Joel Hernandez</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ET-12</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>On Time</t>
-        </is>
-      </c>
+          <t>440236</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>06:50 AM</t>
+          <t>(832) 620-7173</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>F-37</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Late</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>07:45 AM</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Linda Miller</t>
+          <t>Vicky Montez</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>F-250</t>
+          <t>200010</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Late</t>
+          <t>vmontez@ragleinc.com</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>09:15 AM</t>
+          <t>(817) 965-9504</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>ET-71</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>06:47 AM</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>James Wilson</t>
+          <t>Jesus Aguirre</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>RAM-1500</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>On Time</t>
-        </is>
-      </c>
+          <t>240220</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>07:05 AM</t>
+          <t>(214) 577-5146</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>HD-91</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>06:59 AM</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Elizabeth Moore</t>
+          <t>Courtney Scasta</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ET-08</t>
+          <t>210072</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>On Time</t>
+          <t>cscasta@ragleinc.com</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>06:45 AM</t>
+          <t>(972) 921-4993</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>F-06</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>06:57 AM</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>David Taylor</t>
+          <t>Jeffrey Weil</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>F-350</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Early Departure</t>
-        </is>
-      </c>
+          <t>240272</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>07:00 AM</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>14:30 PM</t>
-        </is>
-      </c>
+          <t>(469) 515-3323</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>RAM-42</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>06:57 AM</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Jennifer Anderson</t>
+          <t>Lester Hernandez Roman</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>RAM-2500</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>On Time</t>
-        </is>
-      </c>
+          <t>240513</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>07:20 AM</t>
+          <t>(214) 603-0372</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>TRK-62</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>06:55 AM</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Charles Thomas</t>
+          <t>John Cruz</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ET-15</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Late</t>
-        </is>
-      </c>
+          <t>440148</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>08:45 AM</t>
+          <t>(832) 870-1460</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>TRK-37</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>06:51 AM</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Barbara Jackson</t>
+          <t>Corey Torgerson</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>F-150</t>
+          <t>230016</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>On Time</t>
+          <t>ctorgerson@ragleinc.com</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>06:55 AM</t>
+          <t>(214) 505-6189</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>TRK-51</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>07:05 AM</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Roger Doddy</t>
+          <t>Robert Chandler III</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>UNMATCHED</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
+          <t>340024</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>(817) 709-0554</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>TRK-36</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>06:58 AM</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Samuel Gonzalez</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>230003</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>sgonzalez@ragleinc.com</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>(817) 705-2066</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>F-05</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>06:56 AM</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Juan Reyes Diaz</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>240068</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>jreyes@ragleinc.com</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>(214) 325-7942</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>F-95</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>06:53 AM</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Mario Vasquez</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>240411</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>(469) 306-5298</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>TRK-91</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Late</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>08:13 AM</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Esteban Bahena</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>240547</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>(281) 704-8598</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>TRK-45</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>06:55 AM</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Ramon Perez</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>240063</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>rperezj@ragleinc.com</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>(469) 544-6771</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>HD-91</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>06:51 AM</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Joseph Rodriguez</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>440093</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>(832) 847-5842</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>RAM-81</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>07:04 AM</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Javier Vasquez JR</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>440437</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>javier3878.jv@gmail.com</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>(832) 703-2159</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>F-26</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>06:50 AM</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Luz Rangel Rodriguez</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>240362</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>(817) 312-2078</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>ET-24</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Late</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>07:59 AM</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Ancelmo Diaz Rosas</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>240422</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>(817) 655-5878</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>ET-39</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Early Departure</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>07:12 AM</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>15:30 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Cynthia Chavez</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>200009</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>cchavez@ragleinc.com</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>(682) 216-7161</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>HD-36</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>07:20 AM</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Miguel Carbajal</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>240129</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>carbajal.a.miguel@icloud.com</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>(469) 585-8440</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>TRK-87</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>06:51 AM</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>David Gonzalez</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>240300</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>(469) 314-6315</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>RAM-93</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Late</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>08:00 AM</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Jesus Hernandez-Gonzalez</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>240316</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>jhernandezgonzalez@ragleinc.com</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>(214) 444-0216</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>ET-44</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>06:55 AM</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Mario Rivera</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>240600</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>(903) 237-9069</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>ET-43</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>06:58 AM</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Martha Lopez-Orozco</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>440065</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>(209) 631-6365</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>HD-72</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>06:58 AM</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Bright Ilochi</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>410027</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>bilochi@ragleinc.com</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>(281) 248-3110</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>F-25</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>06:48 AM</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Luis Figueroa-Vazquez</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>440254</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>(281) 748-7253</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>HD-86</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>06:51 AM</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Juan Contreras</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>240359</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>(214) 723-9560</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>HD-32</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>06:49 AM</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Heriberto Garcia JR</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>240708</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>heribertogarciajr222@gmail.com</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>(281) 780-0583</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>HD-02</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>07:07 AM</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Jovani Nunez</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>440239</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>(713) 515-9349</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>F-26</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>07:01 AM</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Fausto Montoya Morales</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>240381</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>montoya.fausto75@gmail.com</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>(817) 357-1665</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>RAM-96</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>06:51 AM</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Ricardo Limon</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>440195</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>(281) 857-2589</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>ET-41</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>06:55 AM</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Juan Cornejo Rosales</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>240001</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>(214) 244-0930</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>F-61</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>06:47 AM</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Hector Bonilla</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>410009</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>hubonilla@ragleinc.com</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>(281) 915-8083</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>HD-87</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>06:54 AM</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Omar Jalomo</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>440025</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>ojalomo@ragleinc.com</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>(956) 564-0649</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>TRK-13</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>06:50 AM</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Juan Hernandez</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>240494</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>juanbhernandez1@aol.com</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>(469) 348-1474</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>HD-45</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Early Departure</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>06:58 AM</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>14:31 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Antonio Delasbour</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>440390</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>antoniodelasbour@yahoo.com</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>(832) 609-7684</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>HD-04</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Late</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>08:02 AM</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>